<commit_message>
Add office option to ets office xls
</commit_message>
<xml_diff>
--- a/public/files/templates/ets-office.xlsx
+++ b/public/files/templates/ets-office.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office</t>
   </si>
 </sst>
 </file>
@@ -274,10 +277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ4"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -344,10 +347,15 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E4" type="list">
-      <formula1>$H$2:$H$4</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E5" type="list">
+      <formula1>$H$2:$H$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>